<commit_message>
Updated excel with results for par vs seq benchmark
</commit_message>
<xml_diff>
--- a/docs/helpers/3.1.3/par_seq_bench.xlsx
+++ b/docs/helpers/3.1.3/par_seq_bench.xlsx
@@ -354,11 +354,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2134711384"/>
-        <c:axId val="2132193224"/>
+        <c:axId val="2115970792"/>
+        <c:axId val="2115973768"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="2134711384"/>
+        <c:axId val="2115970792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -368,7 +368,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2132193224"/>
+        <c:crossAx val="2115973768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -376,7 +376,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2132193224"/>
+        <c:axId val="2115973768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -387,7 +387,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2134711384"/>
+        <c:crossAx val="2115970792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -766,10 +766,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P30"/>
+  <dimension ref="A1:Q30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+      <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -777,7 +777,7 @@
     <col min="16" max="16" width="27.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16" customHeight="1">
+    <row r="1" spans="1:17" ht="16" customHeight="1">
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -785,7 +785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:17">
       <c r="A2">
         <v>1000</v>
       </c>
@@ -796,7 +796,7 @@
         <v>4.8070000000000004</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:17">
       <c r="A3">
         <v>5000</v>
       </c>
@@ -807,7 +807,7 @@
         <v>24.742999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:17">
       <c r="A4">
         <v>10000</v>
       </c>
@@ -818,7 +818,7 @@
         <v>48.823</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:17">
       <c r="A5">
         <v>50000</v>
       </c>
@@ -829,7 +829,7 @@
         <v>249.83500000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:17">
       <c r="A6">
         <v>100000</v>
       </c>
@@ -839,8 +839,14 @@
       <c r="C6">
         <v>491.32600000000002</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="P6">
+        <v>69.665000000000006</v>
+      </c>
+      <c r="Q6">
+        <v>7.7560000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
       <c r="A7">
         <v>250000</v>
       </c>
@@ -850,8 +856,14 @@
       <c r="C7">
         <v>1279.9110000000001</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="P7">
+        <v>63.83</v>
+      </c>
+      <c r="Q7">
+        <v>7.4249999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
       <c r="A8">
         <v>500000</v>
       </c>
@@ -861,8 +873,14 @@
       <c r="C8">
         <v>2543.0680000000002</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="P8">
+        <v>73.980999999999995</v>
+      </c>
+      <c r="Q8">
+        <v>9.8859999999999992</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
       <c r="A9">
         <v>1000000</v>
       </c>
@@ -872,8 +890,14 @@
       <c r="C9">
         <v>5096.2550000000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="P9">
+        <v>69.688000000000002</v>
+      </c>
+      <c r="Q9">
+        <v>7.5309999999999997</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
       <c r="A10">
         <v>2000000</v>
       </c>
@@ -883,8 +907,14 @@
       <c r="C10">
         <v>10187.251</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="P10">
+        <v>75.709999999999994</v>
+      </c>
+      <c r="Q10">
+        <v>7.9059999999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
       <c r="A11">
         <v>4000000</v>
       </c>
@@ -894,8 +924,14 @@
       <c r="C11">
         <v>20381.346000000001</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="P11">
+        <v>72.152000000000001</v>
+      </c>
+      <c r="Q11">
+        <v>8.5670000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
       <c r="A12">
         <v>8000000</v>
       </c>
@@ -904,6 +940,86 @@
       </c>
       <c r="C12">
         <v>40795.784</v>
+      </c>
+      <c r="P12">
+        <v>69.549000000000007</v>
+      </c>
+      <c r="Q12">
+        <v>6.093</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
+      <c r="P13">
+        <v>65.337000000000003</v>
+      </c>
+      <c r="Q13">
+        <v>7.4790000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
+      <c r="P14">
+        <v>64.015000000000001</v>
+      </c>
+      <c r="Q14">
+        <v>6.9619999999999997</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17">
+      <c r="P15">
+        <v>65.867000000000004</v>
+      </c>
+      <c r="Q15">
+        <v>6.4580000000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="16:16">
+      <c r="P17">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="18" spans="16:16">
+      <c r="P18">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="16:16">
+      <c r="P19">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="16:16">
+      <c r="P20">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="21" spans="16:16">
+      <c r="P21">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="16:16">
+      <c r="P22">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="16:16">
+      <c r="P23">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="16:16">
+      <c r="P24">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="25" spans="16:16">
+      <c r="P25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="16:16">
+      <c r="P26">
+        <v>60</v>
       </c>
     </row>
     <row r="30" spans="16:16" ht="405">

</xml_diff>